<commit_message>
fix complex_delivery query args
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
+++ b/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2040" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="1"/>
+    <workbookView xWindow="18180" yWindow="3160" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -414,9 +414,6 @@
     <t>entitlements</t>
   </si>
   <si>
-    <t>['COMPLETE', data('first_last_name'), data('entitlement_id')]</t>
-  </si>
-  <si>
     <t>receive_signature</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t xml:space="preserve">_savepoint_type = ? and _id = ? </t>
+  </si>
+  <si>
+    <t>['COMPLETE', data('entitlement_id')]</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1387,10 @@
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>114</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>115</v>
       </c>
       <c r="G19" s="49"/>
       <c r="H19" s="50"/>
@@ -1456,15 +1456,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>117</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1505,7 +1505,7 @@
         <v>103</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>104</v>
@@ -1537,10 +1537,10 @@
         <v>112</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>113</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>9</v>
@@ -1637,7 +1637,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
change is_delivered to boolean
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
+++ b/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18180" yWindow="3160" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="1"/>
+    <workbookView xWindow="8280" yWindow="3160" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>type</t>
   </si>
@@ -334,9 +334,6 @@
   return str;
   } 
 })()</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
   <si>
     <t>complex_delivery</t>
@@ -1060,7 +1057,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1145,13 +1142,13 @@
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" s="48"/>
       <c r="G4" s="49"/>
@@ -1383,14 +1380,14 @@
       <c r="A19" s="45"/>
       <c r="B19" s="46"/>
       <c r="C19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>113</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>114</v>
       </c>
       <c r="G19" s="49"/>
       <c r="H19" s="50"/>
@@ -1409,8 +1406,8 @@
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
       <c r="H20" s="50"/>
-      <c r="I20" s="56" t="s">
-        <v>87</v>
+      <c r="I20" s="56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1456,15 +1453,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1478,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1496,60 +1493,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="22" t="s">
         <v>107</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>112</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1562,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,7 +1599,7 @@
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -1621,7 +1618,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
@@ -1629,15 +1626,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
@@ -1645,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -1710,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="10"/>
     </row>
@@ -1728,7 +1725,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="10"/>
     </row>
@@ -2030,7 +2027,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
@@ -2038,55 +2035,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
change is_delivered back to string
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
+++ b/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="3160" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="9"/>
+    <workbookView xWindow="4220" yWindow="1960" windowWidth="42920" windowHeight="25120" tabRatio="430" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="123">
   <si>
     <t>type</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>"TRUE"</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1066,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1412,8 +1415,8 @@
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
       <c r="H20" s="50"/>
-      <c r="I20" s="56" t="b">
-        <v>1</v>
+      <c r="I20" s="56" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1439,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1575,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1615,7 +1618,7 @@
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix the bar code range calculation
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
+++ b/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="80" windowWidth="25600" windowHeight="16060" tabRatio="430" activeTab="2"/>
+    <workbookView xWindow="1440" yWindow="80" windowWidth="25600" windowHeight="16060" tabRatio="430"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>end if</t>
   </si>
   <si>
-    <t>!data('valid')</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t>get_itempack</t>
+  </si>
+  <si>
+    <t>!data('valid') || data('valid') == 'false'</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -606,17 +606,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -637,7 +626,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -659,11 +648,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1061,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1071,391 +1059,391 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="36.5" style="31" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="30.5" style="31" customWidth="1"/>
-    <col min="6" max="6" width="88.5" style="31" customWidth="1"/>
-    <col min="7" max="7" width="21" style="31" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="31" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="31" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="31"/>
+    <col min="1" max="1" width="19.6640625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="36.5" style="30" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="30.5" style="30" customWidth="1"/>
+    <col min="6" max="6" width="88.5" style="30" customWidth="1"/>
+    <col min="7" max="7" width="21" style="30" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="23.5" style="30" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="30" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="A2" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="32"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="35" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="41" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="47" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50"/>
-      <c r="J4" s="31" t="b">
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
+      <c r="J4" s="30" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="47" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="50"/>
-      <c r="J5" s="31" t="b">
+      <c r="E5" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="J5" s="30" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="45"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="44"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
+      <c r="I7" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="44"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="45"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="49"/>
-      <c r="I7" s="31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="45"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="45"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="J9" s="31" t="b">
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="J9" s="30" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="51" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="47" t="s">
+      <c r="D10" s="50"/>
+      <c r="E10" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50"/>
-      <c r="J10" s="31" t="b">
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="J10" s="30" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K10" s="46"/>
+      <c r="K10" s="45"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="45"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="51" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="47" t="s">
+      <c r="D11" s="50"/>
+      <c r="E11" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="31" t="s">
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="31" t="b">
+      <c r="J11" s="30" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="53"/>
+    </row>
+    <row r="14" spans="1:11" ht="40">
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="54"/>
-    </row>
-    <row r="14" spans="1:11" ht="40">
-      <c r="A14" s="45"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="51" t="s">
+      <c r="D14" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="47" t="s">
+      <c r="F14" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="31" t="b">
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="30" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="54"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="55"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="45" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="54"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="54"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="54"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="44"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="50"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="55"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="45" t="s">
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="54"/>
+    </row>
+    <row r="20" spans="1:9" ht="23">
+      <c r="A20" s="44"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="54"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="50"/>
+      <c r="E21" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="55"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="55"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="45"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="49"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:9" ht="23">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="55"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="45"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="54"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1485,34 +1473,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="45">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1546,90 +1534,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="22" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
+      <c r="C2" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="D2" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="I2" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="G3" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>107</v>
-      </c>
       <c r="I3" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1647,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1706,7 +1694,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23">
@@ -1714,15 +1702,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="23">
       <c r="A8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>110</v>
+        <v>95</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="23">
@@ -1737,21 +1725,21 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="23">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="23">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="b">
@@ -1759,11 +1747,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="23">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>122</v>
+      <c r="B12" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1811,7 +1799,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="10"/>
     </row>
@@ -1829,7 +1817,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="10"/>
     </row>
@@ -1839,7 +1827,7 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
@@ -1999,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2011,7 +1999,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
@@ -2019,18 +2007,18 @@
     </row>
     <row r="2" spans="1:2" ht="270">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="270">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2063,13 +2051,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
@@ -2080,30 +2068,30 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -2114,19 +2102,19 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2155,66 +2143,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>88</v>
+      <c r="B7" s="17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
complex_delivery has undefined summary field - changed to string
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
+++ b/appGreece/config/tables/complex_delivery/forms/complex_delivery/complex_delivery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="80" windowWidth="25600" windowHeight="16060" tabRatio="430"/>
+    <workbookView xWindow="1440" yWindow="80" windowWidth="25600" windowHeight="16060" tabRatio="430" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="124">
   <si>
     <t>type</t>
   </si>
@@ -545,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -614,8 +614,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -625,8 +636,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -701,16 +716,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1049,7 +1070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1059,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1633,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1755,6 +1776,14 @@
       </c>
       <c r="C12" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23">
+      <c r="A13" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1987,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>